<commit_message>
8 indicadores cap 2
Se completo 8 indicadores del cap 2, estan pendientes 2 indicadores sobre anticoncepción.
</commit_message>
<xml_diff>
--- a/Codigo/Bases/datos_administrativos/Indicadores_de_Género/SALUD/Casos VIHSIDA 2018 AL 2023.xlsx
+++ b/Codigo/Bases/datos_administrativos/Indicadores_de_Género/SALUD/Casos VIHSIDA 2018 AL 2023.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eeovalle\Documents\GitHub\CompendioGenero2023\Codigo\Bases\datos_administrativos\Indicadores_de_Género\SALUD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://inegobgt-my.sharepoint.com/personal/unidadgenero_ine_gob_gt/Documents/Documentos/Github/CompendioGenero2023/Codigo/Bases/datos_administrativos/Indicadores_de_Género/SALUD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{83D4714E-5149-4710-B4AC-B3D7695AF97E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="8_{83D4714E-5149-4710-B4AC-B3D7695AF97E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B7EE30EF-B5C5-47E3-BAF6-18E44A9CD556}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3A84418C-4DB7-4E6C-8747-A2409A35A63B}"/>
+    <workbookView minimized="1" xWindow="3720" yWindow="3720" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{3A84418C-4DB7-4E6C-8747-A2409A35A63B}"/>
   </bookViews>
   <sheets>
     <sheet name="VIHSIDA 2018 al 2023" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="28">
   <si>
     <t>Número de personas notioficadas con VIH/SIDA, por sexo, y edad de los años 2018 al 2023</t>
   </si>
@@ -206,10 +206,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -531,8 +531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B237FB01-1F74-42F7-AB11-A9645D7C7CBC}">
   <dimension ref="B2:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H44" sqref="H44"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -542,15 +542,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
+      <c r="B2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
@@ -562,17 +562,17 @@
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
       <c r="E4" s="2"/>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -773,17 +773,17 @@
       <c r="H14" s="2"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
       <c r="E15" s="2"/>
-      <c r="F15" s="8" t="s">
+      <c r="F15" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
@@ -984,17 +984,17 @@
       <c r="H25" s="2"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="8" t="s">
+      <c r="B26" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
       <c r="E26" s="2"/>
-      <c r="F26" s="8" t="s">
+      <c r="F26" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
@@ -1202,10 +1202,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{597BFFC7-8F2E-4CFF-BB45-6F7F4FC6DF7A}">
-  <dimension ref="B2:M41"/>
+  <dimension ref="B2:Q41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6:Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1217,7 +1217,7 @@
     <col min="7" max="7" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:17" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="9" t="s">
         <v>18</v>
       </c>
@@ -1233,7 +1233,7 @@
       <c r="L2" s="9"/>
       <c r="M2" s="9"/>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B5" s="6">
         <v>2018</v>
       </c>
@@ -1243,7 +1243,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>19</v>
       </c>
@@ -1262,8 +1262,23 @@
       <c r="G6" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="M6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q6" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>25</v>
       </c>
@@ -1282,8 +1297,26 @@
       <c r="G7" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="L7" s="6">
+        <v>2018</v>
+      </c>
+      <c r="M7" s="1">
+        <v>112</v>
+      </c>
+      <c r="N7" s="1">
+        <v>68</v>
+      </c>
+      <c r="O7" s="1">
+        <v>0</v>
+      </c>
+      <c r="P7" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
         <v>26</v>
       </c>
@@ -1302,8 +1335,26 @@
       <c r="G8" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="L8" s="6">
+        <v>2019</v>
+      </c>
+      <c r="M8" s="1">
+        <v>123</v>
+      </c>
+      <c r="N8" s="1">
+        <v>51</v>
+      </c>
+      <c r="O8" s="1">
+        <v>0</v>
+      </c>
+      <c r="P8" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
         <v>27</v>
       </c>
@@ -1322,8 +1373,26 @@
       <c r="G9" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="L9" s="6">
+        <v>2020</v>
+      </c>
+      <c r="M9" s="1">
+        <v>111</v>
+      </c>
+      <c r="N9" s="1">
+        <v>35</v>
+      </c>
+      <c r="O9" s="1">
+        <v>0</v>
+      </c>
+      <c r="P9" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
         <v>12</v>
       </c>
@@ -1342,13 +1411,51 @@
       <c r="G10" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="L10" s="6">
+        <v>2021</v>
+      </c>
+      <c r="M10" s="1">
+        <v>105</v>
+      </c>
+      <c r="N10" s="1">
+        <v>30</v>
+      </c>
+      <c r="O10" s="1">
+        <v>0</v>
+      </c>
+      <c r="P10" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="L11" s="6">
+        <v>2022</v>
+      </c>
+      <c r="M11" s="1">
+        <v>83</v>
+      </c>
+      <c r="N11" s="1">
+        <v>20</v>
+      </c>
+      <c r="O11" s="1">
+        <v>0</v>
+      </c>
+      <c r="P11" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B12" s="6">
         <v>2019</v>
       </c>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
         <v>19</v>
       </c>
@@ -1368,7 +1475,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
         <v>25</v>
       </c>
@@ -1388,7 +1495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
         <v>26</v>
       </c>
@@ -1408,7 +1515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
         <v>27</v>
       </c>

</xml_diff>